<commit_message>
Now calculating the thread URL.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -436,11 +436,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -10091,11 +10095,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -12498,11 +12506,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Views</t>
+        </is>
       </c>
     </row>
     <row r="2">

</xml_diff>